<commit_message>
0206 diary update wenchia
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AD2656-BF14-0B4D-B2AC-9C72FE6BA886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482CD74D-16CB-8F41-B51A-ABC3A3E0D684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -334,6 +334,54 @@
   </si>
   <si>
     <t>Feel Great!</t>
+  </si>
+  <si>
+    <t>20:00 - 21:00</t>
+  </si>
+  <si>
+    <t>To determine 2 features of homework 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussed different features, we finally decided to use 'add new queries' and 'encryption' as our features.  </t>
+  </si>
+  <si>
+    <t>Learned how to use customers' or programmers' perspective to determine which features are needed to be updated.</t>
+  </si>
+  <si>
+    <t>Feel good!</t>
+  </si>
+  <si>
+    <t>To finish research of two features</t>
+  </si>
+  <si>
+    <t>Finished homework 2</t>
+  </si>
+  <si>
+    <t>1. Learned how to explain how to trace code to other group members.
+2. Learned how to understand and explain code to the team members.
+3. Learned how to write down my thought and understanding of the code.</t>
+  </si>
+  <si>
+    <t>Feel exhausted!</t>
+  </si>
+  <si>
+    <t>10:00 - 14:30</t>
+  </si>
+  <si>
+    <t>To read individual homework of week 4</t>
+  </si>
+  <si>
+    <t>1. Understood how UML diagram and Sequence Diagram work
+2. Tried examples in the Youtube videos</t>
+  </si>
+  <si>
+    <t>Learned how to use tools to draw UML and Sequence diagrams</t>
+  </si>
+  <si>
+    <t>Feel Proud!</t>
+  </si>
+  <si>
+    <t>13:00 - 14:30</t>
   </si>
 </sst>
 </file>
@@ -492,7 +540,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +604,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -878,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -890,24 +947,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1366,32 +1423,74 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-    </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
+    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>43865</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="22">
+        <v>43865</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>43867</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
@@ -2229,24 +2328,6 @@
       <c r="E121" s="20"/>
       <c r="F121" s="20"/>
       <c r="G121" s="21"/>
-    </row>
-    <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="20"/>
-      <c r="E122" s="20"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="21"/>
-    </row>
-    <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
-      <c r="D123" s="20"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="20"/>
-      <c r="G123" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
0210 update diary, wen-chia
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482CD74D-16CB-8F41-B51A-ABC3A3E0D684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDD82C6-7635-9340-B102-895C13EA03AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -382,6 +382,22 @@
   </si>
   <si>
     <t>13:00 - 14:30</t>
+  </si>
+  <si>
+    <t>1. Review homework 2 of group project
+2. Understand the concept of KEP and mental simulation.
+3. Midterm Review
+4. Industrial sharing</t>
+  </si>
+  <si>
+    <t>1. Understood KEP and metal simulation.
+2. Had a basic idea of the midterm</t>
+  </si>
+  <si>
+    <t>Learned how KEP concepts are important</t>
+  </si>
+  <si>
+    <t>Feel nervous because of the midterm! Feel not well-prepared for understanding every concept of previous lectures.</t>
   </si>
 </sst>
 </file>
@@ -937,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1492,14 +1508,28 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
+    <row r="29" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>43867</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>

</xml_diff>

<commit_message>
diary update wenchia 0227
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752BF801-AD53-2742-A401-8408C56FF109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BCD52-F255-E548-A157-DCB13AC16870}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="19760" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="188">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -570,6 +570,69 @@
   </si>
   <si>
     <t>After explainning every detail toward relating classes in our essential feature 1, I feel more understanding toward how Real database work when creating table and using table.</t>
+  </si>
+  <si>
+    <t>To think about about how to analyse architecture of the Realm</t>
+  </si>
+  <si>
+    <t>Find very few data about this</t>
+  </si>
+  <si>
+    <t>I used key word 'database architecture' for googling, but most results are related to 3-tier architecture. They are not what we want. Still workiing on it.</t>
+  </si>
+  <si>
+    <t>Feel unhappy!</t>
+  </si>
+  <si>
+    <t>To distribute the small tasks for every group members of assignment 4</t>
+  </si>
+  <si>
+    <t>Finish my part for finding 5 interesting issues.</t>
+  </si>
+  <si>
+    <t>I spent a lot of time tracing every discussions in one issue. Some are interesting because developers might propse nice solutions. Others are someone who don't understand deeply and just wanna answers. They might not be a real issue.</t>
+  </si>
+  <si>
+    <t>Feel intersting!</t>
+  </si>
+  <si>
+    <t>To understand the structure of a database</t>
+  </si>
+  <si>
+    <t>Have a basic understanding of how components work in a database</t>
+  </si>
+  <si>
+    <t>21:00 - 24:00</t>
+  </si>
+  <si>
+    <t>To understand the architecture of realm-core project</t>
+  </si>
+  <si>
+    <t>Have sucessfully understand the fundemental architecture of realm-core</t>
+  </si>
+  <si>
+    <t>I asked my roomate who took a database course last quarter to get a basic understand of components in a database. He gave me some keyword and references to study. It's really helpful, and I finally can understand the code structure in the realm-cre project.</t>
+  </si>
+  <si>
+    <t>We had some debates for some components in our project, but we finally had a conclusion toward the project. Interestingly, when we know nothing about the architecture, we thought a database is too hard for us. After we had a blueprint for understanding the project stucture, it became clearer to us.</t>
+  </si>
+  <si>
+    <t>Feel proud!</t>
+  </si>
+  <si>
+    <t>Feel relief!</t>
+  </si>
+  <si>
+    <t>13:00 - 15:00</t>
+  </si>
+  <si>
+    <t>To integrate every part into final assignment 4</t>
+  </si>
+  <si>
+    <t>Have successfully finished the assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We found how to cowork together everytime we finished the assignment. Even though we think every assignment is still not that easy, we still have ourr way to finish it. </t>
   </si>
 </sst>
 </file>
@@ -737,7 +800,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -818,6 +881,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1140,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2017,50 +2086,120 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="21"/>
-    </row>
-    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="21"/>
-    </row>
-    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="21"/>
-    </row>
-    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="21"/>
-    </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="21"/>
+    <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>43886</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>43886</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>43887</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A46" s="28">
+        <v>43887</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>43888</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>

</xml_diff>

<commit_message>
wenchia update diary 0316
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AC44C0-A871-CB4D-97C7-2A3B53E9DF92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE27D62B-C9E9-6441-8A0E-688B56D9F7F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="254">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -81,9 +81,6 @@
 2. Successfully ran one of two sample open source projects</t>
   </si>
   <si>
-    <t>1. Learned how to solve errors while importing a project</t>
-  </si>
-  <si>
     <t>I was shocked while building Jedit project because I haven't use ant to build my project before. After I bulit it, I got  tons of errors, and I have no idea where to begin fix them.</t>
   </si>
   <si>
@@ -98,11 +95,6 @@
   <si>
     <t>1. Successfully built and ran jedit
 2. Successfully built and ran google guava</t>
-  </si>
-  <si>
-    <t>1. Learned how to use ant build
-2. Learned how to use marven build
-3. Learned how to understand error message after built the project and tried to google it with more precise keywords</t>
   </si>
   <si>
     <t>I tried multiple times to build jedit. Even though I think this project is a little bit outdated, I still enjoy the joy after successfully running it.</t>
@@ -697,6 +689,160 @@
   </si>
   <si>
     <t>This time, I implemented with the pattern by myself and made up some real world situations. Factory patterns are useful and thet often implemented by many application. I'm not unfamiliar with them.</t>
+  </si>
+  <si>
+    <t>To integrate every part into final assignment 5</t>
+  </si>
+  <si>
+    <t>Successfully finished homework 5</t>
+  </si>
+  <si>
+    <t>To find singleton pattern in realm-java and try to figure out the relative relations</t>
+  </si>
+  <si>
+    <t>To find builder pattern in realm-java and try to figure out the relative relations</t>
+  </si>
+  <si>
+    <t>Successfully understood the relation inside the code</t>
+  </si>
+  <si>
+    <t>It was not that hard to find the singleton pattern but to dive more deep into the code to understand the relations was the harder part.</t>
+  </si>
+  <si>
+    <t>Feel tired!</t>
+  </si>
+  <si>
+    <t>We had already traced this part from our assignment 1, so it's quickly for me to understand the relation of the code in this pattern.</t>
+  </si>
+  <si>
+    <t>Feel great!</t>
+  </si>
+  <si>
+    <t>After integrating all patterns inside of our  assignment, I understand the entire codebase clearner than before. Now, I am not afraid of the codebase that much compare to the week 1.</t>
+  </si>
+  <si>
+    <t>1. Review homework 5 of group project
+2. Understand the concept of KEP and testing
+3. Industrial sharing</t>
+  </si>
+  <si>
+    <t>Feel tense!</t>
+  </si>
+  <si>
+    <t>18:00 - 20:00</t>
+  </si>
+  <si>
+    <t>To finish first PR of our project</t>
+  </si>
+  <si>
+    <t>Successful submit the PR</t>
+  </si>
+  <si>
+    <t>We already found several issues on our pocket, and we also did some research for all of them. Even so, we still had stuck in the beginning because we had to use kotlin to revise this issue for the current master branch(latest stable version). Luckily, we switched back to the older java version, and tried to write java code in that version because we found developers didn't change the feature that we want to change since the older version. They just updated code from java to kotlin. Finally, we used IDE for generating kotlin code from Java to finish this PR. This was good because Intellij is so intellogent that can directly generate kotlin code from Java.</t>
+  </si>
+  <si>
+    <t>Feel released.</t>
+  </si>
+  <si>
+    <t>1. From readign test cases of Jpacman I learned that developers should provide documents for test cases. It is because in the test code, sometimes we cannot understand why developers write these code, we could just guess it. So, I think if we can read some instructions of test case, we can understand the code quickly.
+2. The guest provided us a good practice chance to read, analyze and understand the code within the short amount of time. Honestly, I was late to understand the pattern of the code. But after I readlize the pipe-and-filter structur, it was easier to understand the code.</t>
+  </si>
+  <si>
+    <t>10:00 - 11:30</t>
+  </si>
+  <si>
+    <t>Finding second pull request</t>
+  </si>
+  <si>
+    <t>Successfully found several pull requests and would discuss to the group member later</t>
+  </si>
+  <si>
+    <t>It was hard for me to decide whether it was a suitable issue for us to make a PR. I saw a lot of dicussions in the issue, some of the issue were posted for many years and they were still opened. I found most of them were too difficult for us because it might affect many aspects. Finally, I choosed 2 possible issues that seemed not that hard.</t>
+  </si>
+  <si>
+    <t>Feel uncertain!</t>
+  </si>
+  <si>
+    <t>1. Discuss the final
+2. Understand the concept of KEP and advanced topics for this class</t>
+  </si>
+  <si>
+    <t>1. Understand the concept of KEP(play the fool, alert to evidence that challenges their theory and adjust to the degree of uncertainty present)
+2. Have concept of testing and its purpose
+3. Practice of reading test code of Jpacman4 and guess information via these code</t>
+  </si>
+  <si>
+    <t>1. Understand the concept of KEP(know when to stop, reassess the landscape and keep learning)
+2. Have concept of advanced topics(history, visualization and refactoring)</t>
+  </si>
+  <si>
+    <t>This was the last course of this quarter and I leaned a lot of KEPs from this course. Actually, I think the last one 'keep learning' is the most important one. We, as a develoepr, need to always learn new technology to adjust ourselves and adapt the fast changing world. I must be better than myself everyday. Thanks professor for teaching us these useful and practical concepts.</t>
+  </si>
+  <si>
+    <t>Integrate notes from slides and review slides from week 6 to week 10</t>
+  </si>
+  <si>
+    <t>Successfully finished interating all slides into my notebook and review all contents.</t>
+  </si>
+  <si>
+    <t>I found that taking notes in the class was really useful because I could remember what the teacher said via my notes. Therefore, I spent 1.5 hour to integrate all notes from 5 classes into my notebook and then I can review all contents with clearer view.</t>
+  </si>
+  <si>
+    <t>Review all slides from week 1 to week 10</t>
+  </si>
+  <si>
+    <t>Successfully reviewed all contents from week 1 to week 10</t>
+  </si>
+  <si>
+    <t>I listed all possible important concepts that might be appeared in the final and reviewed them again and again. This time I can connect all KEP and I can understand deeply compare to the beginning of the class. Even though some concepts were a little bit confuse, I found that some questions were asked in the Slack, and I got an very clear answer there. It made me understand more about this class.</t>
+  </si>
+  <si>
+    <t>1. To code our second issue 
+2. To identify existing test cases and write new test cases</t>
+  </si>
+  <si>
+    <t>Successfully finished all test cases part of the howeork 6, but still struggling modifying code of the issue</t>
+  </si>
+  <si>
+    <t>Feel complicated!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that we are somehow familiar with the system, we quickly spot three existing test cases and added three test cases into our homework. I think we can clearly understand how the purpose and functions of these test cases. But we are extremely struggling the issue. We tried different ways to implement but it still cannot fulfill our expectation. </t>
+  </si>
+  <si>
+    <t>10:00 - 13:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To code our second issue </t>
+  </si>
+  <si>
+    <t>Not at all, still find relationships in the code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After drawing a diagram of tracing every call related to our second issue, we still somehow got stuck, but at least we now some clue that we can use. So we continue to look official ducument to find more clues. </t>
+  </si>
+  <si>
+    <t>Feel hopeless!</t>
+  </si>
+  <si>
+    <t>We finally understand the restriction of the current codebase. Then we try to think out of box. For realm-java, it cannot allowed us to send proper parameters to the native c++ code to get the expected result. We instead modified the result by implementing different logic to fulfill our goal. We all not sure whether our methods are 100% correct or not, but we follow the coding convention of realm-java and also write test cases for all of our modification.</t>
+  </si>
+  <si>
+    <t>Feel relax!</t>
+  </si>
+  <si>
+    <t>In the class practice, I learned how to solve errors while building a open source project. Because Jedit use different build system that I don't use before, so I google it and also asked TA to solve all errors.</t>
+  </si>
+  <si>
+    <t>1. Learned how to use ant build
+2. Learned how to use maven build
+3. Learned how to understand error message after built the project and tried to google it with more precise keywords</t>
+  </si>
+  <si>
+    <t>Successfully finished the second issue and  write test cases for that. Also, we finish all reports for homework 6.</t>
+  </si>
+  <si>
+    <t>15:00 - 20:30</t>
   </si>
 </sst>
 </file>
@@ -796,7 +942,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -816,6 +962,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -864,7 +1016,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -949,6 +1101,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1273,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1283,24 +1444,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1391,7 +1552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>43839</v>
       </c>
@@ -1399,7 +1560,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>15</v>
@@ -1408,10 +1569,10 @@
         <v>16</v>
       </c>
       <c r="F10" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1419,22 +1580,22 @@
         <v>43846</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="F11" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="136" x14ac:dyDescent="0.2">
@@ -1442,22 +1603,22 @@
         <v>43846</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1465,22 +1626,22 @@
         <v>43847</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="F13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -1488,22 +1649,22 @@
         <v>43849</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="F14" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="G14" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -1511,22 +1672,22 @@
         <v>43849</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="G15" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -1534,22 +1695,22 @@
         <v>43850</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="G16" s="16" t="s">
         <v>48</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="272" x14ac:dyDescent="0.2">
@@ -1557,22 +1718,22 @@
         <v>43854</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="G17" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="136" x14ac:dyDescent="0.2">
@@ -1580,22 +1741,22 @@
         <v>43858</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="G18" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1603,22 +1764,22 @@
         <v>43859</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="E19" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="F19" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="G19" s="18" t="s">
         <v>58</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1626,22 +1787,22 @@
         <v>43859</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="19" t="s">
+      <c r="G20" s="18" t="s">
         <v>62</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1649,22 +1810,22 @@
         <v>43859</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1672,22 +1833,22 @@
         <v>43860</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="19" t="s">
+      <c r="E22" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>74</v>
-      </c>
       <c r="G22" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="272" x14ac:dyDescent="0.2">
@@ -1695,22 +1856,22 @@
         <v>43860</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1718,22 +1879,22 @@
         <v>43860</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="19" t="s">
+      <c r="G24" s="18" t="s">
         <v>86</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -1741,22 +1902,22 @@
         <v>43860</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="F25" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="18" t="s">
         <v>91</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -1764,22 +1925,22 @@
         <v>43865</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="G26" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1787,22 +1948,22 @@
         <v>43865</v>
       </c>
       <c r="B27" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="G27" s="21" t="s">
         <v>96</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1810,22 +1971,22 @@
         <v>43867</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D28" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="G28" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1833,22 +1994,22 @@
         <v>43867</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="G29" s="18" t="s">
         <v>110</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -1856,22 +2017,22 @@
         <v>43874</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E30" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="18" t="s">
         <v>114</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1879,22 +2040,22 @@
         <v>43879</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="E31" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="F31" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="G31" s="26" t="s">
         <v>120</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1902,22 +2063,22 @@
         <v>43879</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="19" t="s">
+      <c r="F32" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="G32" s="18" t="s">
         <v>125</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1925,22 +2086,22 @@
         <v>43880</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="19" t="s">
+      <c r="F33" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>131</v>
-      </c>
       <c r="G33" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1948,22 +2109,22 @@
         <v>43880</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C34" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="F34" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>135</v>
-      </c>
       <c r="G34" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1971,22 +2132,22 @@
         <v>43880</v>
       </c>
       <c r="B35" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="19" t="s">
+      <c r="F35" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="E35" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>139</v>
-      </c>
       <c r="G35" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1994,22 +2155,22 @@
         <v>43881</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="E36" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>142</v>
-      </c>
       <c r="G36" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -2017,22 +2178,22 @@
         <v>43881</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F37" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>145</v>
-      </c>
       <c r="G37" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -2040,22 +2201,22 @@
         <v>43881</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D38" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="E38" s="19" t="s">
-        <v>149</v>
-      </c>
       <c r="F38" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -2063,22 +2224,22 @@
         <v>43881</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="G39" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -2086,22 +2247,22 @@
         <v>43882</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>157</v>
-      </c>
       <c r="F40" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -2109,22 +2270,22 @@
         <v>43883</v>
       </c>
       <c r="B41" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="19" t="s">
+      <c r="F41" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="E41" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>162</v>
-      </c>
       <c r="G41" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -2132,22 +2293,22 @@
         <v>43883</v>
       </c>
       <c r="B42" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="19" t="s">
+      <c r="F42" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="E42" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>166</v>
-      </c>
       <c r="G42" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -2155,22 +2316,22 @@
         <v>43886</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="F43" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="G43" s="18" t="s">
         <v>168</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -2178,22 +2339,22 @@
         <v>43886</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="E44" s="19" t="s">
+      <c r="G44" s="18" t="s">
         <v>172</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -2201,22 +2362,22 @@
         <v>43887</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -2224,22 +2385,22 @@
         <v>43887</v>
       </c>
       <c r="B46" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="E46" s="25" t="s">
+      <c r="F46" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="F46" s="25" t="s">
-        <v>181</v>
-      </c>
       <c r="G46" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -2247,22 +2408,22 @@
         <v>43888</v>
       </c>
       <c r="B47" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E47" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C47" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="19" t="s">
+      <c r="F47" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="E47" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>187</v>
-      </c>
       <c r="G47" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="136" x14ac:dyDescent="0.2">
@@ -2270,22 +2431,22 @@
         <v>43888</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="F48" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="E48" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>190</v>
-      </c>
       <c r="G48" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -2293,22 +2454,22 @@
         <v>43889</v>
       </c>
       <c r="B49" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="19" t="s">
+      <c r="F49" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="E49" s="19" t="s">
+      <c r="G49" s="18" t="s">
         <v>193</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="G49" s="18" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -2316,22 +2477,22 @@
         <v>43890</v>
       </c>
       <c r="B50" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="E50" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="19" t="s">
+      <c r="F50" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="E50" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="F50" s="19" t="s">
-        <v>199</v>
-      </c>
       <c r="G50" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -2339,22 +2500,22 @@
         <v>43891</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D51" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F51" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="E51" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>202</v>
-      </c>
       <c r="G51" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -2362,131 +2523,299 @@
         <v>43892</v>
       </c>
       <c r="B52" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="E52" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="C52" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="19" t="s">
+      <c r="F52" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="G52" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="E52" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F52" s="20" t="s">
+    </row>
+    <row r="53" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A53" s="29">
+        <v>43893</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A54" s="30">
+        <v>43894</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="306" x14ac:dyDescent="0.2">
+      <c r="A55" s="30">
+        <v>43894</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="G55" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A56" s="30">
+        <v>43895</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="E56" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="G52" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="21"/>
-    </row>
-    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="21"/>
-    </row>
-    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="21"/>
-    </row>
-    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="21"/>
-    </row>
-    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="21"/>
-    </row>
-    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="21"/>
-    </row>
-    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="21"/>
-    </row>
-    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="21"/>
-    </row>
-    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="21"/>
-    </row>
-    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="21"/>
-    </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="21"/>
-    </row>
-    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="21"/>
+      <c r="F56" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A57" s="30">
+        <v>43895</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A58" s="30">
+        <v>43902</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A59" s="30">
+        <v>43902</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A60" s="30">
+        <v>43903</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A61" s="30">
+        <v>43905</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A62" s="30">
+        <v>43905</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A63" s="30">
+        <v>43906</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+      <c r="A64" s="30">
+        <v>43906</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="17"/>

</xml_diff>